<commit_message>
Adding extent Reporting Functionality and Screenshots on failTestCases
</commit_message>
<xml_diff>
--- a/Framework_Maven/ObjectRep/ObjectRep.xlsx
+++ b/Framework_Maven/ObjectRep/ObjectRep.xlsx
@@ -470,73 +470,73 @@
     <t>success-container-zip-ext</t>
   </si>
   <si>
+    <t>lblSubmitSuccessMsg</t>
+  </si>
+  <si>
+    <t>btnCloseSubmitSuccess</t>
+  </si>
+  <si>
+    <t>//button[@class='close']</t>
+  </si>
+  <si>
+    <t>//div[contains(text(),'SUCCESS')]</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>IsMultiple</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>loginBtn</t>
+  </si>
+  <si>
+    <t>linkFeatures</t>
+  </si>
+  <si>
+    <t>linkSignUp</t>
+  </si>
+  <si>
+    <t>SignUpPage</t>
+  </si>
+  <si>
+    <t>//input[@value='Login']</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Sign Up</t>
+  </si>
+  <si>
+    <t>Pricing</t>
+  </si>
+  <si>
+    <t>linkPricing</t>
+  </si>
+  <si>
+    <t>paymentPlan</t>
+  </si>
+  <si>
+    <t>payment_plan_id</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>testMultiple</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>username</t>
-  </si>
-  <si>
-    <t>lblSubmitSuccessMsg</t>
-  </si>
-  <si>
-    <t>btnCloseSubmitSuccess</t>
-  </si>
-  <si>
-    <t>//button[@class='close']</t>
-  </si>
-  <si>
-    <t>//div[contains(text(),'SUCCESS')]</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>IsMultiple</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>userName</t>
-  </si>
-  <si>
-    <t>loginBtn</t>
-  </si>
-  <si>
-    <t>linkFeatures</t>
-  </si>
-  <si>
-    <t>linkSignUp</t>
-  </si>
-  <si>
-    <t>SignUpPage</t>
-  </si>
-  <si>
-    <t>//input[@value='Login']</t>
-  </si>
-  <si>
-    <t>Features</t>
-  </si>
-  <si>
-    <t>Sign Up</t>
-  </si>
-  <si>
-    <t>Pricing</t>
-  </si>
-  <si>
-    <t>linkPricing</t>
-  </si>
-  <si>
-    <t>paymentPlan</t>
-  </si>
-  <si>
-    <t>payment_plan_id</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>testMultiple</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -1100,9 +1100,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1123,7 +1123,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -1137,16 +1137,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1157,7 +1157,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>1</v>
@@ -1171,16 +1171,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1188,16 +1188,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1205,16 +1205,16 @@
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1222,16 +1222,16 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1243,53 +1243,53 @@
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>172</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>173</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1319,7 +1319,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>8</v>
@@ -1336,7 +1336,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
@@ -1353,7 +1353,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>8</v>
@@ -1370,7 +1370,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
@@ -1387,7 +1387,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>8</v>
@@ -1404,7 +1404,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>8</v>
@@ -1421,7 +1421,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>61</v>
@@ -1438,7 +1438,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>8</v>
@@ -1455,7 +1455,7 @@
         <v>112</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>8</v>
@@ -1472,7 +1472,7 @@
         <v>113</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>8</v>
@@ -1489,7 +1489,7 @@
         <v>114</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>8</v>
@@ -1506,7 +1506,7 @@
         <v>116</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>8</v>
@@ -1523,7 +1523,7 @@
         <v>115</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>8</v>
@@ -1540,7 +1540,7 @@
         <v>117</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>8</v>
@@ -1557,7 +1557,7 @@
         <v>118</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>8</v>
@@ -1574,7 +1574,7 @@
         <v>119</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>8</v>
@@ -1591,7 +1591,7 @@
         <v>120</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>8</v>
@@ -1608,7 +1608,7 @@
         <v>121</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>8</v>
@@ -1625,7 +1625,7 @@
         <v>122</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>8</v>
@@ -1642,7 +1642,7 @@
         <v>123</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>8</v>
@@ -1659,7 +1659,7 @@
         <v>136</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>8</v>
@@ -1676,7 +1676,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>8</v>
@@ -1693,7 +1693,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>8</v>
@@ -1710,7 +1710,7 @@
         <v>21</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>0</v>
@@ -1727,7 +1727,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>8</v>
@@ -1744,7 +1744,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>8</v>
@@ -1761,7 +1761,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>8</v>
@@ -1778,7 +1778,7 @@
         <v>25</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>8</v>
@@ -1795,7 +1795,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>8</v>
@@ -1812,7 +1812,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>8</v>
@@ -1829,7 +1829,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>8</v>
@@ -1846,7 +1846,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>8</v>
@@ -1863,7 +1863,7 @@
         <v>30</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>8</v>
@@ -1880,7 +1880,7 @@
         <v>31</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>8</v>
@@ -1897,7 +1897,7 @@
         <v>32</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>8</v>
@@ -1914,7 +1914,7 @@
         <v>137</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>8</v>
@@ -1931,7 +1931,7 @@
         <v>33</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>8</v>
@@ -1948,7 +1948,7 @@
         <v>34</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>8</v>
@@ -1965,7 +1965,7 @@
         <v>35</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>8</v>
@@ -1982,7 +1982,7 @@
         <v>36</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>8</v>
@@ -1999,7 +1999,7 @@
         <v>37</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>8</v>
@@ -2016,7 +2016,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>8</v>
@@ -2033,7 +2033,7 @@
         <v>39</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>8</v>
@@ -2050,7 +2050,7 @@
         <v>40</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>8</v>
@@ -2067,7 +2067,7 @@
         <v>41</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>8</v>
@@ -2084,7 +2084,7 @@
         <v>42</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>8</v>
@@ -2101,7 +2101,7 @@
         <v>43</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>8</v>
@@ -2118,7 +2118,7 @@
         <v>44</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>8</v>
@@ -2135,7 +2135,7 @@
         <v>45</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>8</v>
@@ -2152,7 +2152,7 @@
         <v>46</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>8</v>
@@ -2169,7 +2169,7 @@
         <v>47</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>8</v>
@@ -2186,7 +2186,7 @@
         <v>48</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>8</v>
@@ -2203,7 +2203,7 @@
         <v>49</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>8</v>
@@ -2220,7 +2220,7 @@
         <v>50</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>8</v>
@@ -2237,7 +2237,7 @@
         <v>51</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>8</v>
@@ -2254,7 +2254,7 @@
         <v>52</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>8</v>
@@ -2271,7 +2271,7 @@
         <v>53</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>8</v>
@@ -2288,7 +2288,7 @@
         <v>54</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>8</v>
@@ -2305,7 +2305,7 @@
         <v>55</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>8</v>
@@ -2322,7 +2322,7 @@
         <v>56</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>8</v>
@@ -2339,7 +2339,7 @@
         <v>57</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>8</v>
@@ -2356,7 +2356,7 @@
         <v>58</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>8</v>
@@ -2373,7 +2373,7 @@
         <v>59</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>8</v>
@@ -2390,7 +2390,7 @@
         <v>60</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>8</v>
@@ -2407,7 +2407,7 @@
         <v>143</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>0</v>
@@ -2424,7 +2424,7 @@
         <v>141</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>8</v>
@@ -2441,7 +2441,7 @@
         <v>147</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>0</v>
@@ -2458,7 +2458,7 @@
         <v>144</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>0</v>
@@ -2475,7 +2475,7 @@
         <v>140</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>8</v>
@@ -2492,7 +2492,7 @@
         <v>149</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>0</v>
@@ -2506,16 +2506,16 @@
         <v>10</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2523,16 +2523,16 @@
         <v>10</v>
       </c>
       <c r="B72" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="C72" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>